<commit_message>
Added example MS/MS spectra to merged_sample, moved MS/MS spectrum column name to parameter
</commit_message>
<xml_diff>
--- a/inst/extdata/HILIC_pos_sample.xlsx
+++ b/inst/extdata/HILIC_pos_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\notame\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E793E57-13F2-4B30-BE59-98B2D67459AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710D53AE-64EF-46AD-A66F-4C743667DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5856" yWindow="2064" windowWidth="34884" windowHeight="20652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="684" yWindow="5712" windowWidth="31068" windowHeight="18804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area_0_20186261710" sheetId="1" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>56.04976:4077 57.05311:725 58.05647:0</t>
   </si>
   <si>
-    <t>28.018 (100), 56.049 (71), 24.422 (19), 56.075 (6), 48.173 (6), 28.04 (4)</t>
-  </si>
-  <si>
     <t>w/o MS2:N-Methylformamide</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>70.06548:6136 71.06883:195 72.07219:975</t>
   </si>
   <si>
-    <t>70.064 (100), 68.05 (9), 44.049 (7), 43.054 (5), 70.284 (2), 70.121 (1)</t>
-  </si>
-  <si>
     <t>w/o MS2:Pyrrolidine</t>
   </si>
   <si>
@@ -1004,6 +998,12 @@
   </si>
   <si>
     <t>Example_project_HILIC_pos_232</t>
+  </si>
+  <si>
+    <t>24.422:50 28.018:252 28.04:10 48.173:16 56.049:167 56.075:17</t>
+  </si>
+  <si>
+    <t>43.054:7 44.049:10 68.05:14 70.064:150 70.121:1 70.284:3</t>
   </si>
 </sst>
 </file>
@@ -1848,10 +1848,13 @@
   <dimension ref="A1:IH1162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="21" max="21" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:242" x14ac:dyDescent="0.3">
       <c r="U1" t="s">
@@ -3922,667 +3925,667 @@
         <v>29</v>
       </c>
       <c r="V4" t="s">
+        <v>105</v>
+      </c>
+      <c r="W4" t="s">
+        <v>106</v>
+      </c>
+      <c r="X4" t="s">
         <v>107</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>108</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>109</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>110</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AB4" t="s">
         <v>111</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AC4" t="s">
         <v>112</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AD4" t="s">
         <v>113</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
         <v>114</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AF4" t="s">
         <v>115</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>116</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>117</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AI4" t="s">
         <v>118</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AJ4" t="s">
         <v>119</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AK4" t="s">
         <v>120</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AL4" t="s">
         <v>121</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AM4" t="s">
         <v>122</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AN4" t="s">
         <v>123</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AO4" t="s">
         <v>124</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AP4" t="s">
         <v>125</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AQ4" t="s">
         <v>126</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AR4" t="s">
         <v>127</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AS4" t="s">
         <v>128</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AT4" t="s">
         <v>129</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AU4" t="s">
         <v>130</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AV4" t="s">
         <v>131</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AW4" t="s">
         <v>132</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AX4" t="s">
         <v>133</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AY4" t="s">
         <v>134</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AZ4" t="s">
         <v>135</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BA4" t="s">
         <v>136</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BB4" t="s">
         <v>137</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BC4" t="s">
         <v>138</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BD4" t="s">
         <v>139</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BE4" t="s">
         <v>140</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BF4" t="s">
         <v>141</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BG4" t="s">
         <v>142</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BH4" t="s">
         <v>143</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BI4" t="s">
         <v>144</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BJ4" t="s">
         <v>145</v>
       </c>
-      <c r="BI4" t="s">
+      <c r="BK4" t="s">
         <v>146</v>
       </c>
-      <c r="BJ4" t="s">
+      <c r="BL4" t="s">
         <v>147</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BM4" t="s">
         <v>148</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BN4" t="s">
         <v>149</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BO4" t="s">
         <v>150</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="BP4" t="s">
         <v>151</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BQ4" t="s">
         <v>152</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BR4" t="s">
         <v>153</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BS4" t="s">
         <v>154</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="BT4" t="s">
         <v>155</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="BU4" t="s">
         <v>156</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BV4" t="s">
         <v>157</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="BW4" t="s">
         <v>158</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="BX4" t="s">
         <v>159</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="BY4" t="s">
         <v>160</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="BZ4" t="s">
         <v>161</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CA4" t="s">
         <v>162</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CB4" t="s">
         <v>163</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CC4" t="s">
         <v>164</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CD4" t="s">
         <v>165</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CE4" t="s">
         <v>166</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CF4" t="s">
         <v>167</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CG4" t="s">
         <v>168</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CH4" t="s">
         <v>169</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CI4" t="s">
         <v>170</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CJ4" t="s">
         <v>171</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CK4" t="s">
         <v>172</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CL4" t="s">
         <v>173</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CM4" t="s">
         <v>174</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CN4" t="s">
         <v>175</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CO4" t="s">
         <v>176</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CP4" t="s">
         <v>177</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CQ4" t="s">
         <v>178</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CR4" t="s">
         <v>179</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CS4" t="s">
         <v>180</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CT4" t="s">
         <v>181</v>
       </c>
-      <c r="CS4" t="s">
+      <c r="CU4" t="s">
         <v>182</v>
       </c>
-      <c r="CT4" t="s">
+      <c r="CV4" t="s">
         <v>183</v>
       </c>
-      <c r="CU4" t="s">
+      <c r="CW4" t="s">
         <v>184</v>
       </c>
-      <c r="CV4" t="s">
+      <c r="CX4" t="s">
         <v>185</v>
       </c>
-      <c r="CW4" t="s">
+      <c r="CY4" t="s">
         <v>186</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="CZ4" t="s">
         <v>187</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="DA4" t="s">
         <v>188</v>
       </c>
-      <c r="CZ4" t="s">
+      <c r="DB4" t="s">
         <v>189</v>
       </c>
-      <c r="DA4" t="s">
+      <c r="DC4" t="s">
         <v>190</v>
       </c>
-      <c r="DB4" t="s">
+      <c r="DD4" t="s">
         <v>191</v>
       </c>
-      <c r="DC4" t="s">
+      <c r="DE4" t="s">
         <v>192</v>
       </c>
-      <c r="DD4" t="s">
+      <c r="DF4" t="s">
         <v>193</v>
       </c>
-      <c r="DE4" t="s">
+      <c r="DG4" t="s">
         <v>194</v>
       </c>
-      <c r="DF4" t="s">
+      <c r="DH4" t="s">
         <v>195</v>
       </c>
-      <c r="DG4" t="s">
+      <c r="DI4" t="s">
         <v>196</v>
       </c>
-      <c r="DH4" t="s">
+      <c r="DJ4" t="s">
         <v>197</v>
       </c>
-      <c r="DI4" t="s">
+      <c r="DK4" t="s">
         <v>198</v>
       </c>
-      <c r="DJ4" t="s">
+      <c r="DL4" t="s">
         <v>199</v>
       </c>
-      <c r="DK4" t="s">
+      <c r="DM4" t="s">
         <v>200</v>
       </c>
-      <c r="DL4" t="s">
+      <c r="DN4" t="s">
         <v>201</v>
       </c>
-      <c r="DM4" t="s">
+      <c r="DO4" t="s">
         <v>202</v>
       </c>
-      <c r="DN4" t="s">
+      <c r="DP4" t="s">
         <v>203</v>
       </c>
-      <c r="DO4" t="s">
+      <c r="DQ4" t="s">
         <v>204</v>
       </c>
-      <c r="DP4" t="s">
+      <c r="DR4" t="s">
         <v>205</v>
       </c>
-      <c r="DQ4" t="s">
+      <c r="DS4" t="s">
         <v>206</v>
       </c>
-      <c r="DR4" t="s">
+      <c r="DT4" t="s">
         <v>207</v>
       </c>
-      <c r="DS4" t="s">
+      <c r="DU4" t="s">
         <v>208</v>
       </c>
-      <c r="DT4" t="s">
+      <c r="DV4" t="s">
         <v>209</v>
       </c>
-      <c r="DU4" t="s">
+      <c r="DW4" t="s">
         <v>210</v>
       </c>
-      <c r="DV4" t="s">
+      <c r="DX4" t="s">
         <v>211</v>
       </c>
-      <c r="DW4" t="s">
+      <c r="DY4" t="s">
         <v>212</v>
       </c>
-      <c r="DX4" t="s">
+      <c r="DZ4" t="s">
         <v>213</v>
       </c>
-      <c r="DY4" t="s">
+      <c r="EA4" t="s">
         <v>214</v>
       </c>
-      <c r="DZ4" t="s">
+      <c r="EB4" t="s">
         <v>215</v>
       </c>
-      <c r="EA4" t="s">
+      <c r="EC4" t="s">
         <v>216</v>
       </c>
-      <c r="EB4" t="s">
+      <c r="ED4" t="s">
         <v>217</v>
       </c>
-      <c r="EC4" t="s">
+      <c r="EE4" t="s">
         <v>218</v>
       </c>
-      <c r="ED4" t="s">
+      <c r="EF4" t="s">
         <v>219</v>
       </c>
-      <c r="EE4" t="s">
+      <c r="EG4" t="s">
         <v>220</v>
       </c>
-      <c r="EF4" t="s">
+      <c r="EH4" t="s">
         <v>221</v>
       </c>
-      <c r="EG4" t="s">
+      <c r="EI4" t="s">
         <v>222</v>
       </c>
-      <c r="EH4" t="s">
+      <c r="EJ4" t="s">
         <v>223</v>
       </c>
-      <c r="EI4" t="s">
+      <c r="EK4" t="s">
         <v>224</v>
       </c>
-      <c r="EJ4" t="s">
+      <c r="EL4" t="s">
         <v>225</v>
       </c>
-      <c r="EK4" t="s">
+      <c r="EM4" t="s">
         <v>226</v>
       </c>
-      <c r="EL4" t="s">
+      <c r="EN4" t="s">
         <v>227</v>
       </c>
-      <c r="EM4" t="s">
+      <c r="EO4" t="s">
         <v>228</v>
       </c>
-      <c r="EN4" t="s">
+      <c r="EP4" t="s">
         <v>229</v>
       </c>
-      <c r="EO4" t="s">
+      <c r="EQ4" t="s">
         <v>230</v>
       </c>
-      <c r="EP4" t="s">
+      <c r="ER4" t="s">
         <v>231</v>
       </c>
-      <c r="EQ4" t="s">
+      <c r="ES4" t="s">
         <v>232</v>
       </c>
-      <c r="ER4" t="s">
+      <c r="ET4" t="s">
         <v>233</v>
       </c>
-      <c r="ES4" t="s">
+      <c r="EU4" t="s">
         <v>234</v>
       </c>
-      <c r="ET4" t="s">
+      <c r="EV4" t="s">
         <v>235</v>
       </c>
-      <c r="EU4" t="s">
+      <c r="EW4" t="s">
         <v>236</v>
       </c>
-      <c r="EV4" t="s">
+      <c r="EX4" t="s">
         <v>237</v>
       </c>
-      <c r="EW4" t="s">
+      <c r="EY4" t="s">
         <v>238</v>
       </c>
-      <c r="EX4" t="s">
+      <c r="EZ4" t="s">
         <v>239</v>
       </c>
-      <c r="EY4" t="s">
+      <c r="FA4" t="s">
         <v>240</v>
       </c>
-      <c r="EZ4" t="s">
+      <c r="FB4" t="s">
         <v>241</v>
       </c>
-      <c r="FA4" t="s">
+      <c r="FC4" t="s">
         <v>242</v>
       </c>
-      <c r="FB4" t="s">
+      <c r="FD4" t="s">
         <v>243</v>
       </c>
-      <c r="FC4" t="s">
+      <c r="FE4" t="s">
         <v>244</v>
       </c>
-      <c r="FD4" t="s">
+      <c r="FF4" t="s">
         <v>245</v>
       </c>
-      <c r="FE4" t="s">
+      <c r="FG4" t="s">
         <v>246</v>
       </c>
-      <c r="FF4" t="s">
+      <c r="FH4" t="s">
         <v>247</v>
       </c>
-      <c r="FG4" t="s">
+      <c r="FI4" t="s">
         <v>248</v>
       </c>
-      <c r="FH4" t="s">
+      <c r="FJ4" t="s">
         <v>249</v>
       </c>
-      <c r="FI4" t="s">
+      <c r="FK4" t="s">
         <v>250</v>
       </c>
-      <c r="FJ4" t="s">
+      <c r="FL4" t="s">
         <v>251</v>
       </c>
-      <c r="FK4" t="s">
+      <c r="FM4" t="s">
         <v>252</v>
       </c>
-      <c r="FL4" t="s">
+      <c r="FN4" t="s">
         <v>253</v>
       </c>
-      <c r="FM4" t="s">
+      <c r="FO4" t="s">
         <v>254</v>
       </c>
-      <c r="FN4" t="s">
+      <c r="FP4" t="s">
         <v>255</v>
       </c>
-      <c r="FO4" t="s">
+      <c r="FQ4" t="s">
         <v>256</v>
       </c>
-      <c r="FP4" t="s">
+      <c r="FR4" t="s">
         <v>257</v>
       </c>
-      <c r="FQ4" t="s">
+      <c r="FS4" t="s">
         <v>258</v>
       </c>
-      <c r="FR4" t="s">
+      <c r="FT4" t="s">
         <v>259</v>
       </c>
-      <c r="FS4" t="s">
+      <c r="FU4" t="s">
         <v>260</v>
       </c>
-      <c r="FT4" t="s">
+      <c r="FV4" t="s">
         <v>261</v>
       </c>
-      <c r="FU4" t="s">
+      <c r="FW4" t="s">
         <v>262</v>
       </c>
-      <c r="FV4" t="s">
+      <c r="FX4" t="s">
         <v>263</v>
       </c>
-      <c r="FW4" t="s">
+      <c r="FY4" t="s">
         <v>264</v>
       </c>
-      <c r="FX4" t="s">
+      <c r="FZ4" t="s">
         <v>265</v>
       </c>
-      <c r="FY4" t="s">
+      <c r="GA4" t="s">
         <v>266</v>
       </c>
-      <c r="FZ4" t="s">
+      <c r="GB4" t="s">
         <v>267</v>
       </c>
-      <c r="GA4" t="s">
+      <c r="GC4" t="s">
         <v>268</v>
       </c>
-      <c r="GB4" t="s">
+      <c r="GD4" t="s">
         <v>269</v>
       </c>
-      <c r="GC4" t="s">
+      <c r="GE4" t="s">
         <v>270</v>
       </c>
-      <c r="GD4" t="s">
+      <c r="GF4" t="s">
         <v>271</v>
       </c>
-      <c r="GE4" t="s">
+      <c r="GG4" t="s">
         <v>272</v>
       </c>
-      <c r="GF4" t="s">
+      <c r="GH4" t="s">
         <v>273</v>
       </c>
-      <c r="GG4" t="s">
+      <c r="GI4" t="s">
         <v>274</v>
       </c>
-      <c r="GH4" t="s">
+      <c r="GJ4" t="s">
         <v>275</v>
       </c>
-      <c r="GI4" t="s">
+      <c r="GK4" t="s">
         <v>276</v>
       </c>
-      <c r="GJ4" t="s">
+      <c r="GL4" t="s">
         <v>277</v>
       </c>
-      <c r="GK4" t="s">
+      <c r="GM4" t="s">
         <v>278</v>
       </c>
-      <c r="GL4" t="s">
+      <c r="GN4" t="s">
         <v>279</v>
       </c>
-      <c r="GM4" t="s">
+      <c r="GO4" t="s">
         <v>280</v>
       </c>
-      <c r="GN4" t="s">
+      <c r="GP4" t="s">
         <v>281</v>
       </c>
-      <c r="GO4" t="s">
+      <c r="GQ4" t="s">
         <v>282</v>
       </c>
-      <c r="GP4" t="s">
+      <c r="GR4" t="s">
         <v>283</v>
       </c>
-      <c r="GQ4" t="s">
+      <c r="GS4" t="s">
         <v>284</v>
       </c>
-      <c r="GR4" t="s">
+      <c r="GT4" t="s">
         <v>285</v>
       </c>
-      <c r="GS4" t="s">
+      <c r="GU4" t="s">
         <v>286</v>
       </c>
-      <c r="GT4" t="s">
+      <c r="GV4" t="s">
         <v>287</v>
       </c>
-      <c r="GU4" t="s">
+      <c r="GW4" t="s">
         <v>288</v>
       </c>
-      <c r="GV4" t="s">
+      <c r="GX4" t="s">
         <v>289</v>
       </c>
-      <c r="GW4" t="s">
+      <c r="GY4" t="s">
         <v>290</v>
       </c>
-      <c r="GX4" t="s">
+      <c r="GZ4" t="s">
         <v>291</v>
       </c>
-      <c r="GY4" t="s">
+      <c r="HA4" t="s">
         <v>292</v>
       </c>
-      <c r="GZ4" t="s">
+      <c r="HB4" t="s">
         <v>293</v>
       </c>
-      <c r="HA4" t="s">
+      <c r="HC4" t="s">
         <v>294</v>
       </c>
-      <c r="HB4" t="s">
+      <c r="HD4" t="s">
         <v>295</v>
       </c>
-      <c r="HC4" t="s">
+      <c r="HE4" t="s">
         <v>296</v>
       </c>
-      <c r="HD4" t="s">
+      <c r="HF4" t="s">
         <v>297</v>
       </c>
-      <c r="HE4" t="s">
+      <c r="HG4" t="s">
         <v>298</v>
       </c>
-      <c r="HF4" t="s">
+      <c r="HH4" t="s">
         <v>299</v>
       </c>
-      <c r="HG4" t="s">
+      <c r="HI4" t="s">
         <v>300</v>
       </c>
-      <c r="HH4" t="s">
+      <c r="HJ4" t="s">
         <v>301</v>
       </c>
-      <c r="HI4" t="s">
+      <c r="HK4" t="s">
         <v>302</v>
       </c>
-      <c r="HJ4" t="s">
+      <c r="HL4" t="s">
         <v>303</v>
       </c>
-      <c r="HK4" t="s">
+      <c r="HM4" t="s">
         <v>304</v>
       </c>
-      <c r="HL4" t="s">
+      <c r="HN4" t="s">
         <v>305</v>
       </c>
-      <c r="HM4" t="s">
+      <c r="HO4" t="s">
         <v>306</v>
       </c>
-      <c r="HN4" t="s">
+      <c r="HP4" t="s">
         <v>307</v>
       </c>
-      <c r="HO4" t="s">
+      <c r="HQ4" t="s">
         <v>308</v>
       </c>
-      <c r="HP4" t="s">
+      <c r="HR4" t="s">
         <v>309</v>
       </c>
-      <c r="HQ4" t="s">
+      <c r="HS4" t="s">
         <v>310</v>
       </c>
-      <c r="HR4" t="s">
+      <c r="HT4" t="s">
         <v>311</v>
       </c>
-      <c r="HS4" t="s">
+      <c r="HU4" t="s">
         <v>312</v>
       </c>
-      <c r="HT4" t="s">
+      <c r="HV4" t="s">
         <v>313</v>
       </c>
-      <c r="HU4" t="s">
+      <c r="HW4" t="s">
         <v>314</v>
       </c>
-      <c r="HV4" t="s">
+      <c r="HX4" t="s">
         <v>315</v>
       </c>
-      <c r="HW4" t="s">
+      <c r="HY4" t="s">
         <v>316</v>
       </c>
-      <c r="HX4" t="s">
+      <c r="HZ4" t="s">
         <v>317</v>
       </c>
-      <c r="HY4" t="s">
+      <c r="IA4" t="s">
         <v>318</v>
       </c>
-      <c r="HZ4" t="s">
+      <c r="IB4" t="s">
         <v>319</v>
       </c>
-      <c r="IA4" t="s">
+      <c r="IC4" t="s">
         <v>320</v>
       </c>
-      <c r="IB4" t="s">
+      <c r="ID4" t="s">
         <v>321</v>
       </c>
-      <c r="IC4" t="s">
+      <c r="IE4" t="s">
         <v>322</v>
       </c>
-      <c r="ID4" t="s">
+      <c r="IF4" t="s">
         <v>323</v>
       </c>
-      <c r="IE4" t="s">
+      <c r="IG4" t="s">
         <v>324</v>
       </c>
-      <c r="IF4" t="s">
+      <c r="IH4" t="s">
         <v>325</v>
-      </c>
-      <c r="IG4" t="s">
-        <v>326</v>
-      </c>
-      <c r="IH4" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:242" x14ac:dyDescent="0.3">
@@ -4632,7 +4635,7 @@
         <v>-1</v>
       </c>
       <c r="S5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T5" t="s">
         <v>35</v>
@@ -5351,7 +5354,7 @@
         <v>-1</v>
       </c>
       <c r="S6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T6" t="s">
         <v>38</v>
@@ -6070,13 +6073,13 @@
         <v>-1</v>
       </c>
       <c r="S7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T7" t="s">
         <v>39</v>
       </c>
       <c r="U7" t="s">
-        <v>40</v>
+        <v>326</v>
       </c>
       <c r="V7">
         <v>566728.5</v>
@@ -6753,7 +6756,7 @@
         <v>60.044400000000003</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
@@ -6765,13 +6768,13 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
         <v>42</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>43</v>
-      </c>
-      <c r="L8" t="s">
-        <v>44</v>
       </c>
       <c r="N8">
         <v>-1</v>
@@ -6789,10 +6792,10 @@
         <v>-1</v>
       </c>
       <c r="S8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="T8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V8">
         <v>107529.9</v>
@@ -7469,7 +7472,7 @@
         <v>60.080300000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
@@ -7481,13 +7484,13 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
         <v>47</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>48</v>
-      </c>
-      <c r="L9" t="s">
-        <v>49</v>
       </c>
       <c r="N9">
         <v>-1</v>
@@ -7505,10 +7508,10 @@
         <v>-1</v>
       </c>
       <c r="S9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V9">
         <v>93238.37</v>
@@ -8185,7 +8188,7 @@
         <v>61.0396</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
@@ -8197,13 +8200,13 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
         <v>52</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>53</v>
-      </c>
-      <c r="L10" t="s">
-        <v>54</v>
       </c>
       <c r="N10">
         <v>-1</v>
@@ -8221,10 +8224,10 @@
         <v>-1</v>
       </c>
       <c r="S10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="T10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V10">
         <v>59640.72</v>
@@ -8901,7 +8904,7 @@
         <v>64.015699999999995</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>31</v>
@@ -8913,13 +8916,13 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
         <v>57</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>58</v>
-      </c>
-      <c r="L11" t="s">
-        <v>59</v>
       </c>
       <c r="N11">
         <v>-1</v>
@@ -8937,10 +8940,10 @@
         <v>-1</v>
       </c>
       <c r="S11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V11">
         <v>41209.14</v>
@@ -9617,7 +9620,7 @@
         <v>64.015799999999999</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>31</v>
@@ -9629,13 +9632,13 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" t="s">
         <v>57</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>58</v>
-      </c>
-      <c r="L12" t="s">
-        <v>59</v>
       </c>
       <c r="N12">
         <v>-1</v>
@@ -9653,10 +9656,10 @@
         <v>-1</v>
       </c>
       <c r="S12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V12">
         <v>19851.16</v>
@@ -10372,10 +10375,10 @@
         <v>-1</v>
       </c>
       <c r="S13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="T13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V13">
         <v>501741.8</v>
@@ -11091,13 +11094,13 @@
         <v>-1</v>
       </c>
       <c r="S14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U14" t="s">
-        <v>64</v>
+        <v>327</v>
       </c>
       <c r="V14">
         <v>74400.13</v>
@@ -11774,7 +11777,7 @@
         <v>72.080799999999996</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>31</v>
@@ -11786,13 +11789,13 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" t="s">
         <v>66</v>
-      </c>
-      <c r="K15" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" t="s">
-        <v>68</v>
       </c>
       <c r="N15">
         <v>-1</v>
@@ -11810,10 +11813,10 @@
         <v>-1</v>
       </c>
       <c r="S15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V15">
         <v>1264974</v>
@@ -12490,13 +12493,13 @@
         <v>74.057900000000004</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
         <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G16">
         <v>0.3049327</v>
@@ -12505,13 +12508,13 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" t="s">
         <v>72</v>
-      </c>
-      <c r="K16" t="s">
-        <v>73</v>
-      </c>
-      <c r="L16" t="s">
-        <v>74</v>
       </c>
       <c r="N16">
         <v>-1</v>
@@ -12529,10 +12532,10 @@
         <v>-1</v>
       </c>
       <c r="S16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="T16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="V16">
         <v>700309.6</v>
@@ -13209,13 +13212,13 @@
         <v>83.049000000000007</v>
       </c>
       <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
         <v>76</v>
-      </c>
-      <c r="E17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" t="s">
-        <v>78</v>
       </c>
       <c r="G17">
         <v>0.79820630000000004</v>
@@ -13224,13 +13227,13 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" t="s">
         <v>79</v>
-      </c>
-      <c r="K17" t="s">
-        <v>80</v>
-      </c>
-      <c r="L17" t="s">
-        <v>81</v>
       </c>
       <c r="N17">
         <v>-1</v>
@@ -13248,10 +13251,10 @@
         <v>-1</v>
       </c>
       <c r="S17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="T17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="V17">
         <v>1166844</v>
@@ -13967,10 +13970,10 @@
         <v>-1</v>
       </c>
       <c r="S18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="T18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="V18">
         <v>230539.9</v>
@@ -14686,10 +14689,10 @@
         <v>-1</v>
       </c>
       <c r="S19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V19">
         <v>28100.83</v>
@@ -15366,7 +15369,7 @@
         <v>84.080699999999993</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -15378,13 +15381,13 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" t="s">
         <v>86</v>
-      </c>
-      <c r="K20" t="s">
-        <v>87</v>
-      </c>
-      <c r="L20" t="s">
-        <v>88</v>
       </c>
       <c r="N20">
         <v>-1</v>
@@ -15402,10 +15405,10 @@
         <v>-1</v>
       </c>
       <c r="S20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="V20">
         <v>90258.77</v>
@@ -16121,10 +16124,10 @@
         <v>-1</v>
       </c>
       <c r="S21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="V21">
         <v>222917.2</v>
@@ -16801,7 +16804,7 @@
         <v>86.096299999999999</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
         <v>31</v>
@@ -16813,13 +16816,13 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" t="s">
         <v>92</v>
-      </c>
-      <c r="K22" t="s">
-        <v>93</v>
-      </c>
-      <c r="L22" t="s">
-        <v>94</v>
       </c>
       <c r="N22">
         <v>-1</v>
@@ -16837,10 +16840,10 @@
         <v>-1</v>
       </c>
       <c r="S22" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="T22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="V22">
         <v>227357.2</v>
@@ -17556,10 +17559,10 @@
         <v>-1</v>
       </c>
       <c r="S23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V23">
         <v>218213</v>
@@ -18236,7 +18239,7 @@
         <v>88.039500000000004</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
         <v>31</v>
@@ -18248,13 +18251,13 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
+        <v>96</v>
+      </c>
+      <c r="K24" t="s">
+        <v>97</v>
+      </c>
+      <c r="L24" t="s">
         <v>98</v>
-      </c>
-      <c r="K24" t="s">
-        <v>99</v>
-      </c>
-      <c r="L24" t="s">
-        <v>100</v>
       </c>
       <c r="N24">
         <v>-1</v>
@@ -18272,10 +18275,10 @@
         <v>-1</v>
       </c>
       <c r="S24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="V24">
         <v>218213</v>
@@ -18952,7 +18955,7 @@
         <v>89.107399999999998</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
         <v>31</v>
@@ -18964,13 +18967,13 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" t="s">
+        <v>102</v>
+      </c>
+      <c r="L25" t="s">
         <v>103</v>
-      </c>
-      <c r="K25" t="s">
-        <v>104</v>
-      </c>
-      <c r="L25" t="s">
-        <v>105</v>
       </c>
       <c r="N25">
         <v>-1</v>
@@ -18988,10 +18991,10 @@
         <v>-1</v>
       </c>
       <c r="S25" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="T25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="V25">
         <v>48543.46</v>
@@ -19872,12 +19875,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20027,15 +20027,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4C25D04-767B-4978-816E-4424818623DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13DB352-349E-442E-A6C7-988FB8BED4D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20059,10 +20063,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D13DB352-349E-442E-A6C7-988FB8BED4D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4C25D04-767B-4978-816E-4424818623DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>